<commit_message>
updated with Identify, Correlate, Measure, Compute
</commit_message>
<xml_diff>
--- a/POI_Development Training_Name/1. Analysis/Developer_Workbook-SOFOR.xlsx
+++ b/POI_Development Training_Name/1. Analysis/Developer_Workbook-SOFOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sacas/pCloud Drive/4DF/Local copy/Library/Knowledge Management/Obsidian Vault/4OSD/Training/Course Development/poi-SOFOR/POI_Development Training_Name/1. Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE77668-2460-1541-B843-2AC5207ADA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6A6AC1-15A4-E34F-BA87-44F7B779B9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="913" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11579,8 +11579,8 @@
   </sheetPr>
   <dimension ref="B1:P659"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>